<commit_message>
update source code for ICO DApp and finished all the content of this project. Also update patterns for tutorials.
</commit_message>
<xml_diff>
--- a/以太坊教程/以太坊课程大纲.xlsx
+++ b/以太坊教程/以太坊课程大纲.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>课程名</t>
   </si>
@@ -142,13 +142,17 @@
   </si>
   <si>
     <t>next.js + react + material-UI + mocha</t>
+  </si>
+  <si>
+    <t>尚硅谷区块链技术——以太坊课程大纲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +182,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -205,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -321,11 +332,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -354,24 +374,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -380,6 +382,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,9 +705,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -694,248 +719,257 @@
     <col min="4" max="4" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="5" t="s">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D4" s="5">
         <v>4</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="6" t="s">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14"/>
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="6">
         <v>5</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="6" t="s">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D7" s="6">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D8" s="5">
         <v>6</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="6" t="s">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="6">
         <v>6</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D10" s="5">
         <v>6</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D12" s="4">
         <v>5</v>
       </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="5" t="s">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D13" s="5">
         <v>4</v>
       </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D14" s="6">
         <v>3</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D15" s="5">
         <v>3</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="50.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D16" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="5" t="s">
+    <row r="17" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D17" s="5">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="6" t="s">
+    <row r="18" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D18" s="6">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A9"/>
+  <mergeCells count="5">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>